<commit_message>
Small fixes in column width
</commit_message>
<xml_diff>
--- a/Altium_Templates/VTEC_BOM_Template.xlsx
+++ b/Altium_Templates/VTEC_BOM_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omar-\Documents\GitHub\VTEC-CAD_LIBRARY\Altium_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEEBBD9-2DA8-4E6F-A264-21D63A61EB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CA0392-164B-4BB2-82F7-C8E9CE2C4AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C3956FD4-1A44-4C90-9B5B-E48BD0F97FB2}"/>
   </bookViews>
@@ -418,7 +418,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -455,8 +455,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -480,45 +478,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -530,14 +536,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -576,16 +582,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>234</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1768</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>671125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1767</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>14076</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>588065</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>154880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -608,8 +614,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16768880" y="1010024"/>
-          <a:ext cx="2169609" cy="583808"/>
+          <a:off x="16880190" y="772050"/>
+          <a:ext cx="2169810" cy="583808"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -921,23 +927,23 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
     <col min="7" max="7" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="24.85546875" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
     <col min="14" max="14" width="9.140625" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
@@ -971,15 +977,15 @@
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="33" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="14"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
@@ -993,17 +999,17 @@
       <c r="D3" s="14"/>
       <c r="E3" s="16"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
     </row>
     <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -1019,11 +1025,11 @@
       <c r="G4" s="19"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="J4" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="K4" s="18"/>
-      <c r="L4" s="18" t="s">
-        <v>30</v>
-      </c>
+      <c r="L4" s="18"/>
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
       <c r="O4" s="20"/>
@@ -1037,20 +1043,20 @@
       <c r="D5" s="21"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="37" t="s">
+      <c r="G5" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="H5" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="35" t="s">
+      <c r="I5" s="18"/>
+      <c r="J5" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
       <c r="O5" s="20"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="20"/>
@@ -1068,14 +1074,14 @@
         <v>7</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
@@ -1086,28 +1092,28 @@
       <c r="C7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="59">
         <f ca="1">TODAY()</f>
         <v>44916</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="60">
         <f ca="1">NOW()</f>
-        <v>44916.647066435187</v>
+        <v>44916.666609490741</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="J7" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="K7" s="18"/>
-      <c r="L7" s="18" t="s">
-        <v>10</v>
-      </c>
+      <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
@@ -1149,120 +1155,120 @@
     </row>
     <row r="10" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="31" t="s">
+      <c r="K10" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="31" t="s">
+      <c r="M10" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="31" t="s">
+      <c r="N10" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="31" t="s">
+      <c r="O10" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="31" t="s">
+      <c r="P10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="31" t="s">
+      <c r="Q10" s="29" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
-      <c r="B11" s="32">
+      <c r="B11" s="30">
         <f>ROW(B11) - ROW($B$10)</f>
         <v>1</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="30"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="33">
+      <c r="B12" s="31">
         <f t="shared" ref="B12:B13" si="0">ROW(B12) - ROW($B$10)</f>
         <v>2</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="31"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="32">
+      <c r="B13" s="30">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="30"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
@@ -1274,61 +1280,61 @@
         <f>SUM(M11:M13)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="34">
+      <c r="P14" s="32">
         <f>SUM(P11:P13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="47"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="57">
+      <c r="D21" s="54"/>
+      <c r="E21" s="36">
         <f>COUNT(B11:B13)</f>
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="58">
+      <c r="D22" s="56"/>
+      <c r="E22" s="37">
         <f>SUMIF($I$11:$I$13, "Surface Mount", $J$11:$J$13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="59">
+      <c r="D23" s="58"/>
+      <c r="E23" s="38">
         <f>SUMIF($I$11:$I$13, "Through Hole", $J$11:$J$13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="56"/>
-      <c r="E24" s="60">
+      <c r="D24" s="41"/>
+      <c r="E24" s="39">
         <f>SUMIF($I$11:$I$13, "Mechanical", $J$11:$J$13)</f>
         <v>0</v>
       </c>
@@ -1357,11 +1363,11 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="J5:L6"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C19:E20"/>
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="L5:N6"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>

</xml_diff>

<commit_message>
Changed quantity column location
</commit_message>
<xml_diff>
--- a/Altium_Templates/VTEC_BOM_Template.xlsx
+++ b/Altium_Templates/VTEC_BOM_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omar-\Documents\GitHub\VTEC-CAD_LIBRARY\Altium_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A3CF15-A9AA-4213-BBDF-477D27E63B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFABD5E-A04B-4569-BFD3-2D1471038936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C3956FD4-1A44-4C90-9B5B-E48BD0F97FB2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Report Date</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>Field=OutputName</t>
+  </si>
+  <si>
+    <t>Column=Case/Package</t>
+  </si>
+  <si>
+    <t>Column=Supplier Subtotal per Board 1</t>
   </si>
 </sst>
 </file>
@@ -418,7 +424,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -499,6 +505,15 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -550,28 +565,7 @@
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Valuta" xfId="2" builtinId="4"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -589,7 +583,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -617,41 +611,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -673,16 +632,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>671125</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>637994</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1767</xdr:rowOff>
+      <xdr:rowOff>18333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>588065</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57978</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>154880</xdr:rowOff>
+      <xdr:rowOff>171446</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -705,7 +664,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16880190" y="772050"/>
+          <a:off x="16979581" y="788616"/>
           <a:ext cx="2169810" cy="583808"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1015,11 +974,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8FD7D1-B5D4-4075-BAF9-23D41E564942}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11:I13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1029,39 +986,43 @@
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="24.85546875" customWidth="1"/>
-    <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="10"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="10"/>
+      <c r="G1" s="9"/>
       <c r="H1" s="10"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="9"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-    </row>
-    <row r="2" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6"/>
       <c r="B2" s="11"/>
       <c r="C2" s="15" t="s">
@@ -1072,38 +1033,42 @@
       <c r="F2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="16"/>
+      <c r="G2" s="33"/>
       <c r="H2" s="16"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="24"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
-    </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="12"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="16"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="27"/>
-    </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+    </row>
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="13"/>
       <c r="C4" s="17" t="s">
@@ -1114,46 +1079,50 @@
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="17"/>
+      <c r="K4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
       <c r="Q4" s="20"/>
-    </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="13"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="53" t="s">
+      <c r="G5" s="18"/>
+      <c r="H5" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="I5" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="44"/>
+      <c r="K5" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="18"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
       <c r="Q5" s="20"/>
-    </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+    </row>
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="13"/>
       <c r="C6" s="18" t="s">
@@ -1166,19 +1135,21 @@
         <v>7</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="59"/>
       <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="18"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
-    </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="14"/>
       <c r="C7" s="18" t="s">
@@ -1186,28 +1157,30 @@
       </c>
       <c r="D7" s="40">
         <f ca="1">TODAY()</f>
-        <v>44916</v>
+        <v>44917</v>
       </c>
       <c r="E7" s="41">
         <f ca="1">NOW()</f>
-        <v>44916.674611805553</v>
+        <v>44917.515682523146</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="18"/>
+      <c r="K7" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="23"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="14"/>
       <c r="C8" s="18"/>
@@ -1225,8 +1198,10 @@
       <c r="O8" s="18"/>
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -1244,8 +1219,10 @@
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
-    </row>
-    <row r="10" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="28" t="s">
         <v>2</v>
@@ -1263,40 +1240,46 @@
         <v>25</v>
       </c>
       <c r="G10" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="I10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="J10" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="29" t="s">
+      <c r="L10" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="29" t="s">
+      <c r="M10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="N10" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="29" t="s">
+      <c r="O10" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="29" t="s">
+      <c r="P10" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="29" t="s">
+      <c r="Q10" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="29" t="s">
+      <c r="S10" s="29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="30">
         <f>ROW(B11) - ROW($B$10)</f>
@@ -1309,16 +1292,18 @@
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="30"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="34"/>
       <c r="L11" s="30"/>
       <c r="M11" s="30"/>
       <c r="N11" s="30"/>
-      <c r="O11" s="42"/>
+      <c r="O11" s="30"/>
       <c r="P11" s="42"/>
-      <c r="Q11" s="30"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="30"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="31">
         <f t="shared" ref="B12:B13" si="0">ROW(B12) - ROW($B$10)</f>
@@ -1331,16 +1316,18 @@
       <c r="G12" s="35"/>
       <c r="H12" s="35"/>
       <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="31"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="35"/>
       <c r="L12" s="31"/>
       <c r="M12" s="31"/>
       <c r="N12" s="31"/>
-      <c r="O12" s="43"/>
+      <c r="O12" s="31"/>
       <c r="P12" s="43"/>
-      <c r="Q12" s="31"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="31"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="30">
         <f t="shared" si="0"/>
@@ -1353,142 +1340,147 @@
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="30"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="34"/>
       <c r="L13" s="30"/>
       <c r="M13" s="30"/>
       <c r="N13" s="30"/>
-      <c r="O13" s="42"/>
+      <c r="O13" s="30"/>
       <c r="P13" s="42"/>
-      <c r="Q13" s="30"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="30"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="J14">
-        <f>SUM(J11:J13)</f>
+      <c r="G14">
+        <f>SUM(G11:G13)</f>
         <v>0</v>
       </c>
-      <c r="M14">
-        <f>SUM(M11:M13)</f>
+      <c r="N14">
+        <f>SUM(N11:N13)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="32">
-        <f>SUM(P11:P13)</f>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="32">
+        <f>SUM(R11:R13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="47" t="s">
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="49"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="57" t="s">
+      <c r="D19" s="51"/>
+      <c r="E19" s="52"/>
+    </row>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="53"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="55"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="58"/>
+      <c r="D21" s="61"/>
       <c r="E21" s="36">
         <f>COUNT(B11:B13)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="59" t="s">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="60"/>
+      <c r="D22" s="63"/>
       <c r="E22" s="37">
-        <f>SUMIF($I$11:$I$13, "Surface Mount", $J$11:$J$13)</f>
+        <f xml:space="preserve"> SUMIF($K$11:$K$13, "Surface Mount",$G$11:$G$13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="62"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="38">
-        <f>SUMIF($I$11:$I$13, "Through Hole", $J$11:$J$13)</f>
+        <f xml:space="preserve"> SUMIF($K$11:$K$13, "Through Hole",$G$11:$G$13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="46"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="39">
-        <f>SUMIF($I$11:$I$13, "Mechanical", $J$11:$J$13)</f>
+        <f xml:space="preserve"> SUMIF($K$11:$K$13, "Mechanical",$G$11:$G$13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="31" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="2"/>
+      <c r="G31" s="1"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
       <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="J5:L6"/>
+    <mergeCell ref="K5:M6"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C19:E20"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
   </mergeCells>
-  <conditionalFormatting sqref="N11:N13">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
+  <conditionalFormatting sqref="O11:O13">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
+      <formula>LEN(TRIM(O11))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="lessThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="8" priority="4">
-      <formula>LEN(TRIM(N11))=0</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R11:R13">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
+      <formula>LEN(TRIM(R11))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P11:P13">
-    <cfRule type="containsBlanks" dxfId="14" priority="6">
-      <formula>LEN(TRIM(P11))=0</formula>
+  <conditionalFormatting sqref="K11:K13">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(K11))=0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11:I13">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Through Hole">
-      <formula>NOT(ISERROR(SEARCH("Through Hole",I11)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Mechanical">
+      <formula>NOT(ISERROR(SEARCH("Mechanical",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Mechanical">
-      <formula>NOT(ISERROR(SEARCH("Mechanical",I11)))</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(I11))=0</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Through Hole">
+      <formula>NOT(ISERROR(SEARCH("Through Hole",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>